<commit_message>
adding lists to xlsx
</commit_message>
<xml_diff>
--- a/PriceList.xlsx
+++ b/PriceList.xlsx
@@ -8,6 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="LCL_FILO_ASIA" sheetId="1" r:id="rId1"/>
+    <sheet name="AUTO_LNR" sheetId="2" r:id="rId2"/>
+    <sheet name="LCL_RAIL_ASIA" sheetId="3" r:id="rId3"/>
+    <sheet name="FCL_ASIA" sheetId="4" r:id="rId4"/>
+    <sheet name="FCL_RAIL_ASIA" sheetId="5" r:id="rId5"/>
+    <sheet name="FCL_AUTO_LNR" sheetId="6" r:id="rId6"/>
+    <sheet name="RAIL_CHINA_LCL" sheetId="7" r:id="rId7"/>
+    <sheet name="RAIL_CHINA_FCL" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -172,6 +179,13 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -180,7 +194,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,7 +240,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,11 +254,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -225,61 +277,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -294,22 +302,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,79 +331,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,103 +505,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,32 +536,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -583,6 +564,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -607,6 +612,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -621,162 +637,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1118,7 +1125,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2111,4 +2118,116 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>